<commit_message>
fixed bugs, added status
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="351">
   <si>
     <t>team</t>
   </si>
@@ -1058,6 +1058,15 @@
   </si>
   <si>
     <t>Glen Perkins</t>
+  </si>
+  <si>
+    <t>David Freese</t>
+  </si>
+  <si>
+    <t>Derek Norris</t>
+  </si>
+  <si>
+    <t>Houston Street</t>
   </si>
 </sst>
 </file>
@@ -1886,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D317"/>
+  <dimension ref="A1:D320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="F291" sqref="F291"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="D171" sqref="D171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,7 +4266,7 @@
         <v>4</v>
       </c>
       <c r="D169" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -6329,6 +6338,48 @@
         <v>4</v>
       </c>
       <c r="D317" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>179</v>
+      </c>
+      <c r="B318" t="s">
+        <v>348</v>
+      </c>
+      <c r="C318">
+        <v>6</v>
+      </c>
+      <c r="D318" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>179</v>
+      </c>
+      <c r="B319" t="s">
+        <v>349</v>
+      </c>
+      <c r="C319">
+        <v>12</v>
+      </c>
+      <c r="D319" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>179</v>
+      </c>
+      <c r="B320" t="s">
+        <v>350</v>
+      </c>
+      <c r="C320">
+        <v>18</v>
+      </c>
+      <c r="D320" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
end of main draft
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="504">
   <si>
     <t>team</t>
   </si>
@@ -1066,9 +1066,6 @@
     <t>Derek Norris</t>
   </si>
   <si>
-    <t>Houston Street</t>
-  </si>
-  <si>
     <t>Bryan Shaw</t>
   </si>
   <si>
@@ -1132,9 +1129,6 @@
     <t>Luke Gregerson</t>
   </si>
   <si>
-    <t>Barolo Colon</t>
-  </si>
-  <si>
     <t>Ryan Zimmerman</t>
   </si>
   <si>
@@ -1379,6 +1373,159 @@
   </si>
   <si>
     <t>Dioner Navarro</t>
+  </si>
+  <si>
+    <t>Angel Pagan</t>
+  </si>
+  <si>
+    <t>James Paxton</t>
+  </si>
+  <si>
+    <t>Justin Masterson</t>
+  </si>
+  <si>
+    <t>Michael Bourn</t>
+  </si>
+  <si>
+    <t>Neil Ramirez</t>
+  </si>
+  <si>
+    <t>Andrew Heaney</t>
+  </si>
+  <si>
+    <t>Joe Smith</t>
+  </si>
+  <si>
+    <t>Adeiny Hechavarria</t>
+  </si>
+  <si>
+    <t>Mike Moustakas</t>
+  </si>
+  <si>
+    <t>Rene Rivera</t>
+  </si>
+  <si>
+    <t>Steven Matz</t>
+  </si>
+  <si>
+    <t>Yusmeiro Petit</t>
+  </si>
+  <si>
+    <t>Kyle Gibson</t>
+  </si>
+  <si>
+    <t>Shane Victorino</t>
+  </si>
+  <si>
+    <t>Anthony Gose</t>
+  </si>
+  <si>
+    <t>Andrelton Simmons</t>
+  </si>
+  <si>
+    <t>DJ LeMahieu</t>
+  </si>
+  <si>
+    <t>Mike Aviles</t>
+  </si>
+  <si>
+    <t>Zach Putnam</t>
+  </si>
+  <si>
+    <t>Drew Pomeranz</t>
+  </si>
+  <si>
+    <t>Tony Watson</t>
+  </si>
+  <si>
+    <t>Yangervis Solarte</t>
+  </si>
+  <si>
+    <t>Nick Hundley</t>
+  </si>
+  <si>
+    <t>Mark Buehrle</t>
+  </si>
+  <si>
+    <t>Kyle Hendricks</t>
+  </si>
+  <si>
+    <t>Kevin Plawecki</t>
+  </si>
+  <si>
+    <t>Tommy Hunter</t>
+  </si>
+  <si>
+    <t>Marcus Semien</t>
+  </si>
+  <si>
+    <t>Brandon Finnegan</t>
+  </si>
+  <si>
+    <t>David Murphy</t>
+  </si>
+  <si>
+    <t>Matt Moore</t>
+  </si>
+  <si>
+    <t>Conor Gillaspie</t>
+  </si>
+  <si>
+    <t>Kevin Quackenbush</t>
+  </si>
+  <si>
+    <t>Chris Johnson</t>
+  </si>
+  <si>
+    <t>Manuel Margot</t>
+  </si>
+  <si>
+    <t>Fernando Abed</t>
+  </si>
+  <si>
+    <t>Darren O'Day</t>
+  </si>
+  <si>
+    <t>Dan Otero</t>
+  </si>
+  <si>
+    <t>Adam Lind</t>
+  </si>
+  <si>
+    <t>Trevor Plouffe</t>
+  </si>
+  <si>
+    <t>Wade Miley</t>
+  </si>
+  <si>
+    <t>Christian Bethancourt</t>
+  </si>
+  <si>
+    <t>Charlie Morton</t>
+  </si>
+  <si>
+    <t>Joe Panik</t>
+  </si>
+  <si>
+    <t>Gerardo Parra</t>
+  </si>
+  <si>
+    <t>Ryan Rua</t>
+  </si>
+  <si>
+    <t>Yasmani Tomas</t>
+  </si>
+  <si>
+    <t>B.J. Upton</t>
+  </si>
+  <si>
+    <t>Huston Street</t>
+  </si>
+  <si>
+    <t>Tim Hudson</t>
+  </si>
+  <si>
+    <t>Bartolo Colon</t>
   </si>
 </sst>
 </file>
@@ -2207,10 +2354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D424"/>
+  <dimension ref="A1:D473"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="D423" sqref="D423"/>
+    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
+      <selection activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2558,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -5891,7 +6038,7 @@
         <v>263</v>
       </c>
       <c r="B263" t="s">
-        <v>295</v>
+        <v>502</v>
       </c>
       <c r="C263">
         <v>4</v>
@@ -6009,7 +6156,7 @@
         <v>4</v>
       </c>
       <c r="D271" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6485,7 +6632,7 @@
         <v>9</v>
       </c>
       <c r="D305" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.25">
@@ -6689,7 +6836,7 @@
         <v>179</v>
       </c>
       <c r="B320" t="s">
-        <v>350</v>
+        <v>501</v>
       </c>
       <c r="C320">
         <v>18</v>
@@ -6703,7 +6850,7 @@
         <v>91</v>
       </c>
       <c r="B321" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C321">
         <v>2</v>
@@ -6717,7 +6864,7 @@
         <v>263</v>
       </c>
       <c r="B322" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C322">
         <v>12</v>
@@ -6731,13 +6878,13 @@
         <v>278</v>
       </c>
       <c r="B323" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C323">
         <v>6</v>
       </c>
       <c r="D323" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -6745,7 +6892,7 @@
         <v>164</v>
       </c>
       <c r="B324" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C324">
         <v>13</v>
@@ -6759,7 +6906,7 @@
         <v>278</v>
       </c>
       <c r="B325" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C325">
         <v>8</v>
@@ -6773,7 +6920,7 @@
         <v>230</v>
       </c>
       <c r="B326" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C326">
         <v>13</v>
@@ -6787,7 +6934,7 @@
         <v>59</v>
       </c>
       <c r="B327" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C327">
         <v>7</v>
@@ -6801,7 +6948,7 @@
         <v>263</v>
       </c>
       <c r="B328" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C328">
         <v>5</v>
@@ -6815,7 +6962,7 @@
         <v>201</v>
       </c>
       <c r="B329" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C329">
         <v>11</v>
@@ -6829,7 +6976,7 @@
         <v>74</v>
       </c>
       <c r="B330" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C330">
         <v>10</v>
@@ -6843,7 +6990,7 @@
         <v>43</v>
       </c>
       <c r="B331" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C331">
         <v>4</v>
@@ -6857,7 +7004,7 @@
         <v>74</v>
       </c>
       <c r="B332" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C332">
         <v>10</v>
@@ -6871,7 +7018,7 @@
         <v>91</v>
       </c>
       <c r="B333" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C333">
         <v>4</v>
@@ -6885,7 +7032,7 @@
         <v>164</v>
       </c>
       <c r="B334" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C334">
         <v>5</v>
@@ -6899,7 +7046,7 @@
         <v>74</v>
       </c>
       <c r="B335" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C335">
         <v>14</v>
@@ -6913,7 +7060,7 @@
         <v>249</v>
       </c>
       <c r="B336" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C336">
         <v>6</v>
@@ -6927,7 +7074,7 @@
         <v>120</v>
       </c>
       <c r="B337" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C337">
         <v>12</v>
@@ -6941,7 +7088,7 @@
         <v>230</v>
       </c>
       <c r="B338" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C338">
         <v>3</v>
@@ -6955,7 +7102,7 @@
         <v>74</v>
       </c>
       <c r="B339" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C339">
         <v>8</v>
@@ -6969,7 +7116,7 @@
         <v>146</v>
       </c>
       <c r="B340" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C340">
         <v>1</v>
@@ -6983,7 +7130,7 @@
         <v>4</v>
       </c>
       <c r="B341" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C341">
         <v>8</v>
@@ -6997,7 +7144,7 @@
         <v>59</v>
       </c>
       <c r="B342" t="s">
-        <v>372</v>
+        <v>503</v>
       </c>
       <c r="C342">
         <v>1</v>
@@ -7011,7 +7158,7 @@
         <v>263</v>
       </c>
       <c r="B343" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C343">
         <v>16</v>
@@ -7025,7 +7172,7 @@
         <v>249</v>
       </c>
       <c r="B344" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C344">
         <v>9</v>
@@ -7039,7 +7186,7 @@
         <v>164</v>
       </c>
       <c r="B345" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C345">
         <v>4</v>
@@ -7053,7 +7200,7 @@
         <v>26</v>
       </c>
       <c r="B346" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C346">
         <v>9</v>
@@ -7067,7 +7214,7 @@
         <v>164</v>
       </c>
       <c r="B347" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C347">
         <v>7</v>
@@ -7081,7 +7228,7 @@
         <v>216</v>
       </c>
       <c r="B348" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C348">
         <v>7</v>
@@ -7095,7 +7242,7 @@
         <v>216</v>
       </c>
       <c r="B349" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C349">
         <v>5</v>
@@ -7109,7 +7256,7 @@
         <v>43</v>
       </c>
       <c r="B350" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C350">
         <v>1</v>
@@ -7123,7 +7270,7 @@
         <v>216</v>
       </c>
       <c r="B351" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C351">
         <v>3</v>
@@ -7137,7 +7284,7 @@
         <v>164</v>
       </c>
       <c r="B352" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C352">
         <v>6</v>
@@ -7151,7 +7298,7 @@
         <v>164</v>
       </c>
       <c r="B353" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C353">
         <v>8</v>
@@ -7165,7 +7312,7 @@
         <v>4</v>
       </c>
       <c r="B354" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C354">
         <v>9</v>
@@ -7179,7 +7326,7 @@
         <v>216</v>
       </c>
       <c r="B355" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C355">
         <v>7</v>
@@ -7193,7 +7340,7 @@
         <v>278</v>
       </c>
       <c r="B356" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C356">
         <v>2</v>
@@ -7207,7 +7354,7 @@
         <v>74</v>
       </c>
       <c r="B357" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C357">
         <v>10</v>
@@ -7221,7 +7368,7 @@
         <v>278</v>
       </c>
       <c r="B358" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C358">
         <v>2</v>
@@ -7235,7 +7382,7 @@
         <v>201</v>
       </c>
       <c r="B359" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C359">
         <v>4</v>
@@ -7249,7 +7396,7 @@
         <v>59</v>
       </c>
       <c r="B360" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C360">
         <v>6</v>
@@ -7263,7 +7410,7 @@
         <v>263</v>
       </c>
       <c r="B361" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C361">
         <v>5</v>
@@ -7277,7 +7424,7 @@
         <v>278</v>
       </c>
       <c r="B362" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C362">
         <v>11</v>
@@ -7291,7 +7438,7 @@
         <v>201</v>
       </c>
       <c r="B363" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C363">
         <v>5</v>
@@ -7305,7 +7452,7 @@
         <v>43</v>
       </c>
       <c r="B364" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C364">
         <v>6</v>
@@ -7319,7 +7466,7 @@
         <v>216</v>
       </c>
       <c r="B365" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C365">
         <v>5</v>
@@ -7333,7 +7480,7 @@
         <v>249</v>
       </c>
       <c r="B366" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C366">
         <v>3</v>
@@ -7347,7 +7494,7 @@
         <v>249</v>
       </c>
       <c r="B367" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C367">
         <v>2</v>
@@ -7361,7 +7508,7 @@
         <v>230</v>
       </c>
       <c r="B368" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C368">
         <v>4</v>
@@ -7375,7 +7522,7 @@
         <v>201</v>
       </c>
       <c r="B369" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C369">
         <v>3</v>
@@ -7389,7 +7536,7 @@
         <v>278</v>
       </c>
       <c r="B370" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C370">
         <v>5</v>
@@ -7403,7 +7550,7 @@
         <v>201</v>
       </c>
       <c r="B371" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C371">
         <v>7</v>
@@ -7417,7 +7564,7 @@
         <v>278</v>
       </c>
       <c r="B372" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C372">
         <v>5</v>
@@ -7431,7 +7578,7 @@
         <v>74</v>
       </c>
       <c r="B373" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C373">
         <v>2</v>
@@ -7445,7 +7592,7 @@
         <v>216</v>
       </c>
       <c r="B374" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C374">
         <v>7</v>
@@ -7459,7 +7606,7 @@
         <v>146</v>
       </c>
       <c r="B375" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C375">
         <v>1</v>
@@ -7473,7 +7620,7 @@
         <v>120</v>
       </c>
       <c r="B376" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C376">
         <v>2</v>
@@ -7487,7 +7634,7 @@
         <v>59</v>
       </c>
       <c r="B377" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C377">
         <v>6</v>
@@ -7501,7 +7648,7 @@
         <v>263</v>
       </c>
       <c r="B378" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C378">
         <v>7</v>
@@ -7515,7 +7662,7 @@
         <v>164</v>
       </c>
       <c r="B379" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C379">
         <v>9</v>
@@ -7529,7 +7676,7 @@
         <v>108</v>
       </c>
       <c r="B380" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C380">
         <v>1</v>
@@ -7543,7 +7690,7 @@
         <v>132</v>
       </c>
       <c r="B381" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C381">
         <v>1</v>
@@ -7557,7 +7704,7 @@
         <v>216</v>
       </c>
       <c r="B382" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C382">
         <v>4</v>
@@ -7571,7 +7718,7 @@
         <v>26</v>
       </c>
       <c r="B383" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C383">
         <v>2</v>
@@ -7585,7 +7732,7 @@
         <v>120</v>
       </c>
       <c r="B384" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C384">
         <v>2</v>
@@ -7599,7 +7746,7 @@
         <v>216</v>
       </c>
       <c r="B385" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C385">
         <v>7</v>
@@ -7613,7 +7760,7 @@
         <v>132</v>
       </c>
       <c r="B386" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C386">
         <v>3</v>
@@ -7627,7 +7774,7 @@
         <v>278</v>
       </c>
       <c r="B387" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C387">
         <v>3</v>
@@ -7641,7 +7788,7 @@
         <v>249</v>
       </c>
       <c r="B388" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C388">
         <v>2</v>
@@ -7655,7 +7802,7 @@
         <v>230</v>
       </c>
       <c r="B389" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C389">
         <v>3</v>
@@ -7669,7 +7816,7 @@
         <v>278</v>
       </c>
       <c r="B390" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C390">
         <v>5</v>
@@ -7683,7 +7830,7 @@
         <v>74</v>
       </c>
       <c r="B391" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C391">
         <v>3</v>
@@ -7697,7 +7844,7 @@
         <v>146</v>
       </c>
       <c r="B392" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C392">
         <v>1</v>
@@ -7711,7 +7858,7 @@
         <v>120</v>
       </c>
       <c r="B393" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C393">
         <v>3</v>
@@ -7725,7 +7872,7 @@
         <v>59</v>
       </c>
       <c r="B394" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C394">
         <v>9</v>
@@ -7739,7 +7886,7 @@
         <v>263</v>
       </c>
       <c r="B395" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C395">
         <v>6</v>
@@ -7753,7 +7900,7 @@
         <v>164</v>
       </c>
       <c r="B396" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C396">
         <v>10</v>
@@ -7767,7 +7914,7 @@
         <v>108</v>
       </c>
       <c r="B397" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C397">
         <v>1</v>
@@ -7781,7 +7928,7 @@
         <v>120</v>
       </c>
       <c r="B398" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C398">
         <v>10</v>
@@ -7795,7 +7942,7 @@
         <v>164</v>
       </c>
       <c r="B399" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C399">
         <v>14</v>
@@ -7809,7 +7956,7 @@
         <v>263</v>
       </c>
       <c r="B400" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C400">
         <v>6</v>
@@ -7823,7 +7970,7 @@
         <v>59</v>
       </c>
       <c r="B401" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C401">
         <v>7</v>
@@ -7837,7 +7984,7 @@
         <v>249</v>
       </c>
       <c r="B402" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C402">
         <v>1</v>
@@ -7851,7 +7998,7 @@
         <v>91</v>
       </c>
       <c r="B403" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C403">
         <v>1</v>
@@ -7865,7 +8012,7 @@
         <v>278</v>
       </c>
       <c r="B404" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C404">
         <v>1</v>
@@ -7879,7 +8026,7 @@
         <v>201</v>
       </c>
       <c r="B405" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C405">
         <v>1</v>
@@ -7893,7 +8040,7 @@
         <v>230</v>
       </c>
       <c r="B406" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C406">
         <v>3</v>
@@ -7907,7 +8054,7 @@
         <v>216</v>
       </c>
       <c r="B407" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C407">
         <v>5</v>
@@ -7921,7 +8068,7 @@
         <v>120</v>
       </c>
       <c r="B408" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C408">
         <v>3</v>
@@ -7935,7 +8082,7 @@
         <v>59</v>
       </c>
       <c r="B409" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C409">
         <v>3</v>
@@ -7949,13 +8096,13 @@
         <v>278</v>
       </c>
       <c r="B410" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C410">
         <v>4</v>
       </c>
       <c r="D410" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.25">
@@ -7963,7 +8110,7 @@
         <v>108</v>
       </c>
       <c r="B411" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C411">
         <v>4</v>
@@ -7977,7 +8124,7 @@
         <v>91</v>
       </c>
       <c r="B412" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C412">
         <v>3</v>
@@ -7991,7 +8138,7 @@
         <v>249</v>
       </c>
       <c r="B413" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C413">
         <v>4</v>
@@ -8005,7 +8152,7 @@
         <v>132</v>
       </c>
       <c r="B414" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C414">
         <v>2</v>
@@ -8019,7 +8166,7 @@
         <v>4</v>
       </c>
       <c r="B415" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C415">
         <v>1</v>
@@ -8033,7 +8180,7 @@
         <v>59</v>
       </c>
       <c r="B416" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C416">
         <v>7</v>
@@ -8047,7 +8194,7 @@
         <v>59</v>
       </c>
       <c r="B417" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C417">
         <v>3</v>
@@ -8061,7 +8208,7 @@
         <v>108</v>
       </c>
       <c r="B418" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C418">
         <v>3</v>
@@ -8075,7 +8222,7 @@
         <v>132</v>
       </c>
       <c r="B419" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C419">
         <v>1</v>
@@ -8089,7 +8236,7 @@
         <v>216</v>
       </c>
       <c r="B420" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C420">
         <v>1</v>
@@ -8103,7 +8250,7 @@
         <v>26</v>
       </c>
       <c r="B421" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C421">
         <v>1</v>
@@ -8117,7 +8264,7 @@
         <v>43</v>
       </c>
       <c r="B422" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C422">
         <v>1</v>
@@ -8128,10 +8275,10 @@
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="B423" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C423">
         <v>3</v>
@@ -8145,13 +8292,699 @@
         <v>108</v>
       </c>
       <c r="B424" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C424">
         <v>3</v>
       </c>
       <c r="D424" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>249</v>
+      </c>
+      <c r="B425" t="s">
+        <v>453</v>
+      </c>
+      <c r="C425">
+        <v>4</v>
+      </c>
+      <c r="D425" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>120</v>
+      </c>
+      <c r="B426" t="s">
+        <v>454</v>
+      </c>
+      <c r="C426">
+        <v>2</v>
+      </c>
+      <c r="D426" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>278</v>
+      </c>
+      <c r="B427" t="s">
+        <v>455</v>
+      </c>
+      <c r="C427">
+        <v>1</v>
+      </c>
+      <c r="D427" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>108</v>
+      </c>
+      <c r="B428" t="s">
+        <v>456</v>
+      </c>
+      <c r="C428">
+        <v>4</v>
+      </c>
+      <c r="D428" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>108</v>
+      </c>
+      <c r="B429" t="s">
+        <v>469</v>
+      </c>
+      <c r="C429">
+        <v>2</v>
+      </c>
+      <c r="D429" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>4</v>
+      </c>
+      <c r="B430" t="s">
+        <v>457</v>
+      </c>
+      <c r="C430">
+        <v>2</v>
+      </c>
+      <c r="D430" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>120</v>
+      </c>
+      <c r="B431" t="s">
+        <v>458</v>
+      </c>
+      <c r="C431">
+        <v>2</v>
+      </c>
+      <c r="D431" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>59</v>
+      </c>
+      <c r="B432" t="s">
+        <v>459</v>
+      </c>
+      <c r="C432">
+        <v>1</v>
+      </c>
+      <c r="D432" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="433" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>164</v>
+      </c>
+      <c r="B433" t="s">
+        <v>460</v>
+      </c>
+      <c r="C433">
+        <v>2</v>
+      </c>
+      <c r="D433" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="434" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>108</v>
+      </c>
+      <c r="B434" t="s">
+        <v>461</v>
+      </c>
+      <c r="C434">
+        <v>2</v>
+      </c>
+      <c r="D434" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="435" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>132</v>
+      </c>
+      <c r="B435" t="s">
+        <v>462</v>
+      </c>
+      <c r="C435">
+        <v>1</v>
+      </c>
+      <c r="D435" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="436" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>26</v>
+      </c>
+      <c r="B436" t="s">
+        <v>463</v>
+      </c>
+      <c r="C436">
+        <v>1</v>
+      </c>
+      <c r="D436" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="437" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>91</v>
+      </c>
+      <c r="B437" t="s">
+        <v>464</v>
+      </c>
+      <c r="C437">
+        <v>1</v>
+      </c>
+      <c r="D437" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="438" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>43</v>
+      </c>
+      <c r="B438" t="s">
+        <v>465</v>
+      </c>
+      <c r="C438">
+        <v>1</v>
+      </c>
+      <c r="D438" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="439" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>278</v>
+      </c>
+      <c r="B439" t="s">
+        <v>466</v>
+      </c>
+      <c r="C439">
+        <v>4</v>
+      </c>
+      <c r="D439" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="440" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>201</v>
+      </c>
+      <c r="B440" t="s">
+        <v>467</v>
+      </c>
+      <c r="C440">
+        <v>1</v>
+      </c>
+      <c r="D440" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="441" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>230</v>
+      </c>
+      <c r="B441" t="s">
+        <v>468</v>
+      </c>
+      <c r="C441">
+        <v>1</v>
+      </c>
+      <c r="D441" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="442" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>91</v>
+      </c>
+      <c r="B442" t="s">
+        <v>470</v>
+      </c>
+      <c r="C442">
+        <v>1</v>
+      </c>
+      <c r="D442" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>4</v>
+      </c>
+      <c r="B443" t="s">
+        <v>471</v>
+      </c>
+      <c r="C443">
+        <v>1</v>
+      </c>
+      <c r="D443" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="444" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>120</v>
+      </c>
+      <c r="B444" t="s">
+        <v>472</v>
+      </c>
+      <c r="C444">
+        <v>1</v>
+      </c>
+      <c r="D444" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>59</v>
+      </c>
+      <c r="B445" t="s">
+        <v>473</v>
+      </c>
+      <c r="C445">
+        <v>5</v>
+      </c>
+      <c r="D445" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="446" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>108</v>
+      </c>
+      <c r="B446" t="s">
+        <v>474</v>
+      </c>
+      <c r="C446">
+        <v>1</v>
+      </c>
+      <c r="D446" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="447" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>132</v>
+      </c>
+      <c r="B447" t="s">
+        <v>475</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+      <c r="D447" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="448" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>108</v>
+      </c>
+      <c r="B448" t="s">
+        <v>476</v>
+      </c>
+      <c r="C448">
+        <v>2</v>
+      </c>
+      <c r="D448" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="449" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>26</v>
+      </c>
+      <c r="B449" t="s">
+        <v>477</v>
+      </c>
+      <c r="C449">
+        <v>1</v>
+      </c>
+      <c r="D449" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="450" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>91</v>
+      </c>
+      <c r="B450" t="s">
+        <v>478</v>
+      </c>
+      <c r="C450">
+        <v>1</v>
+      </c>
+      <c r="D450" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="451" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>4</v>
+      </c>
+      <c r="B451" t="s">
+        <v>479</v>
+      </c>
+      <c r="C451">
+        <v>1</v>
+      </c>
+      <c r="D451" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="452" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>120</v>
+      </c>
+      <c r="B452" t="s">
+        <v>480</v>
+      </c>
+      <c r="C452">
+        <v>1</v>
+      </c>
+      <c r="D452" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="453" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>108</v>
+      </c>
+      <c r="B453" t="s">
+        <v>481</v>
+      </c>
+      <c r="C453">
+        <v>1</v>
+      </c>
+      <c r="D453" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="454" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>132</v>
+      </c>
+      <c r="B454" t="s">
+        <v>482</v>
+      </c>
+      <c r="C454">
+        <v>1</v>
+      </c>
+      <c r="D454" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="455" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>132</v>
+      </c>
+      <c r="B455" t="s">
+        <v>483</v>
+      </c>
+      <c r="C455">
+        <v>3</v>
+      </c>
+      <c r="D455" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="456" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>91</v>
+      </c>
+      <c r="B456" t="s">
+        <v>484</v>
+      </c>
+      <c r="C456">
+        <v>1</v>
+      </c>
+      <c r="D456" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="457" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>4</v>
+      </c>
+      <c r="B457" t="s">
+        <v>485</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+      <c r="D457" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="458" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>132</v>
+      </c>
+      <c r="B458" t="s">
+        <v>486</v>
+      </c>
+      <c r="C458">
+        <v>1</v>
+      </c>
+      <c r="D458" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="459" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>91</v>
+      </c>
+      <c r="B459" t="s">
+        <v>487</v>
+      </c>
+      <c r="C459">
+        <v>1</v>
+      </c>
+      <c r="D459" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="460" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>4</v>
+      </c>
+      <c r="B460" t="s">
+        <v>488</v>
+      </c>
+      <c r="C460">
+        <v>1</v>
+      </c>
+      <c r="D460" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="461" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>4</v>
+      </c>
+      <c r="B461" t="s">
+        <v>489</v>
+      </c>
+      <c r="C461">
+        <v>1</v>
+      </c>
+      <c r="D461" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="462" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>4</v>
+      </c>
+      <c r="B462" t="s">
+        <v>490</v>
+      </c>
+      <c r="C462">
+        <v>1</v>
+      </c>
+      <c r="D462" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="463" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>164</v>
+      </c>
+      <c r="B463" t="s">
+        <v>491</v>
+      </c>
+      <c r="C463">
+        <v>1</v>
+      </c>
+      <c r="D463" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="464" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>164</v>
+      </c>
+      <c r="B464" t="s">
+        <v>492</v>
+      </c>
+      <c r="C464">
+        <v>1</v>
+      </c>
+      <c r="D464" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="465" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>164</v>
+      </c>
+      <c r="B465" t="s">
+        <v>493</v>
+      </c>
+      <c r="C465">
+        <v>1</v>
+      </c>
+      <c r="D465" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="466" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>43</v>
+      </c>
+      <c r="B466" t="s">
+        <v>494</v>
+      </c>
+      <c r="C466">
+        <v>1</v>
+      </c>
+      <c r="D466" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="467" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>43</v>
+      </c>
+      <c r="B467" t="s">
+        <v>378</v>
+      </c>
+      <c r="C467">
+        <v>1</v>
+      </c>
+      <c r="D467" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="468" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>108</v>
+      </c>
+      <c r="B468" t="s">
+        <v>495</v>
+      </c>
+      <c r="C468">
+        <v>1</v>
+      </c>
+      <c r="D468" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="469" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>59</v>
+      </c>
+      <c r="B469" t="s">
+        <v>496</v>
+      </c>
+      <c r="C469">
+        <v>2</v>
+      </c>
+      <c r="D469" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="470" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>59</v>
+      </c>
+      <c r="B470" t="s">
+        <v>497</v>
+      </c>
+      <c r="C470">
+        <v>3</v>
+      </c>
+      <c r="D470" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="471" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>120</v>
+      </c>
+      <c r="B471" t="s">
+        <v>498</v>
+      </c>
+      <c r="C471">
+        <v>2</v>
+      </c>
+      <c r="D471" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="472" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>201</v>
+      </c>
+      <c r="B472" t="s">
+        <v>499</v>
+      </c>
+      <c r="C472">
+        <v>17</v>
+      </c>
+      <c r="D472" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="473" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>146</v>
+      </c>
+      <c r="B473" t="s">
+        <v>500</v>
+      </c>
+      <c r="C473">
+        <v>8</v>
+      </c>
+      <c r="D473" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start of bench draft
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="527">
   <si>
     <t>team</t>
   </si>
@@ -1526,6 +1526,75 @@
   </si>
   <si>
     <t>Bartolo Colon</t>
+  </si>
+  <si>
+    <t>Jesse Winker</t>
+  </si>
+  <si>
+    <t>Jonathan Schoop</t>
+  </si>
+  <si>
+    <t>Mitch Moreland</t>
+  </si>
+  <si>
+    <t>Michael Taylor</t>
+  </si>
+  <si>
+    <t>Matt Olson</t>
+  </si>
+  <si>
+    <t>Jordan Walden</t>
+  </si>
+  <si>
+    <t>Eric Young</t>
+  </si>
+  <si>
+    <t>Kyle Schwarber</t>
+  </si>
+  <si>
+    <t>David Dejesus</t>
+  </si>
+  <si>
+    <t>Steven Moya</t>
+  </si>
+  <si>
+    <t>Patrick Corbin</t>
+  </si>
+  <si>
+    <t>Nick Swisher</t>
+  </si>
+  <si>
+    <t>Daniel Norris</t>
+  </si>
+  <si>
+    <t>Michael Conforto</t>
+  </si>
+  <si>
+    <t>Wilmer Flores</t>
+  </si>
+  <si>
+    <t>Jose Peraza</t>
+  </si>
+  <si>
+    <t>Jeurys Familia</t>
+  </si>
+  <si>
+    <t>Ichiro Suzuki</t>
+  </si>
+  <si>
+    <t>Josh Johnson</t>
+  </si>
+  <si>
+    <t>Luis Severino</t>
+  </si>
+  <si>
+    <t>Jameson Taillon</t>
+  </si>
+  <si>
+    <t>Cody Asche</t>
+  </si>
+  <si>
+    <t>Ike Davis</t>
   </si>
 </sst>
 </file>
@@ -2354,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D473"/>
+  <dimension ref="A1:D496"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="D326" sqref="D326"/>
+    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
+      <selection activeCell="C475" sqref="C475:C496"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8987,7 +9056,330 @@
         <v>6</v>
       </c>
     </row>
+    <row r="474" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>4</v>
+      </c>
+      <c r="B474" t="s">
+        <v>504</v>
+      </c>
+      <c r="C474">
+        <v>0</v>
+      </c>
+      <c r="D474" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="475" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>216</v>
+      </c>
+      <c r="B475" t="s">
+        <v>505</v>
+      </c>
+      <c r="C475">
+        <v>0</v>
+      </c>
+      <c r="D475" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="476" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>108</v>
+      </c>
+      <c r="B476" t="s">
+        <v>506</v>
+      </c>
+      <c r="C476">
+        <v>0</v>
+      </c>
+      <c r="D476" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="477" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>278</v>
+      </c>
+      <c r="B477" t="s">
+        <v>507</v>
+      </c>
+      <c r="C477">
+        <v>0</v>
+      </c>
+      <c r="D477" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="478" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>120</v>
+      </c>
+      <c r="B478" t="s">
+        <v>508</v>
+      </c>
+      <c r="C478">
+        <v>0</v>
+      </c>
+      <c r="D478" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="479" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>120</v>
+      </c>
+      <c r="B479" t="s">
+        <v>509</v>
+      </c>
+      <c r="C479">
+        <v>0</v>
+      </c>
+      <c r="D479" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="480" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>43</v>
+      </c>
+      <c r="B480" t="s">
+        <v>510</v>
+      </c>
+      <c r="C480">
+        <v>0</v>
+      </c>
+      <c r="D480" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="481" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>201</v>
+      </c>
+      <c r="B481" t="s">
+        <v>511</v>
+      </c>
+      <c r="C481">
+        <v>0</v>
+      </c>
+      <c r="D481" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="482" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>278</v>
+      </c>
+      <c r="B482" t="s">
+        <v>512</v>
+      </c>
+      <c r="C482">
+        <v>0</v>
+      </c>
+      <c r="D482" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="483" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>26</v>
+      </c>
+      <c r="B483" t="s">
+        <v>513</v>
+      </c>
+      <c r="C483">
+        <v>0</v>
+      </c>
+      <c r="D483" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="484" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>249</v>
+      </c>
+      <c r="B484" t="s">
+        <v>514</v>
+      </c>
+      <c r="C484">
+        <v>0</v>
+      </c>
+      <c r="D484" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="485" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>146</v>
+      </c>
+      <c r="B485" t="s">
+        <v>515</v>
+      </c>
+      <c r="C485">
+        <v>0</v>
+      </c>
+      <c r="D485" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="486" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>216</v>
+      </c>
+      <c r="B486" t="s">
+        <v>516</v>
+      </c>
+      <c r="C486">
+        <v>0</v>
+      </c>
+      <c r="D486" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="487" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>4</v>
+      </c>
+      <c r="B487" t="s">
+        <v>517</v>
+      </c>
+      <c r="C487">
+        <v>0</v>
+      </c>
+      <c r="D487" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="488" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>4</v>
+      </c>
+      <c r="B488" t="s">
+        <v>518</v>
+      </c>
+      <c r="C488">
+        <v>0</v>
+      </c>
+      <c r="D488" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="489" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>216</v>
+      </c>
+      <c r="B489" t="s">
+        <v>519</v>
+      </c>
+      <c r="C489">
+        <v>0</v>
+      </c>
+      <c r="D489" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="490" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>108</v>
+      </c>
+      <c r="B490" t="s">
+        <v>520</v>
+      </c>
+      <c r="C490">
+        <v>0</v>
+      </c>
+      <c r="D490" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="491" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>108</v>
+      </c>
+      <c r="B491" t="s">
+        <v>521</v>
+      </c>
+      <c r="C491">
+        <v>0</v>
+      </c>
+      <c r="D491" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="492" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>249</v>
+      </c>
+      <c r="B492" t="s">
+        <v>522</v>
+      </c>
+      <c r="C492">
+        <v>0</v>
+      </c>
+      <c r="D492" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="493" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>26</v>
+      </c>
+      <c r="B493" t="s">
+        <v>523</v>
+      </c>
+      <c r="C493">
+        <v>0</v>
+      </c>
+      <c r="D493" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="494" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>230</v>
+      </c>
+      <c r="B494" t="s">
+        <v>524</v>
+      </c>
+      <c r="C494">
+        <v>0</v>
+      </c>
+      <c r="D494" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="495" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>74</v>
+      </c>
+      <c r="B495" t="s">
+        <v>525</v>
+      </c>
+      <c r="C495">
+        <v>0</v>
+      </c>
+      <c r="D495" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="496" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>278</v>
+      </c>
+      <c r="B496" t="s">
+        <v>526</v>
+      </c>
+      <c r="C496">
+        <v>0</v>
+      </c>
+      <c r="D496" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
switched in depth chart projections
</commit_message>
<xml_diff>
--- a/draftpicks.xlsx
+++ b/draftpicks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="610">
   <si>
     <t>team</t>
   </si>
@@ -1513,9 +1513,6 @@
     <t>Ryan Rua</t>
   </si>
   <si>
-    <t>Yasmani Tomas</t>
-  </si>
-  <si>
     <t>B.J. Upton</t>
   </si>
   <si>
@@ -1769,6 +1766,84 @@
   </si>
   <si>
     <t>Jose Iglesias</t>
+  </si>
+  <si>
+    <t>Anthony DeSclafini</t>
+  </si>
+  <si>
+    <t>Darin Ruf</t>
+  </si>
+  <si>
+    <t>Jesse Chavez</t>
+  </si>
+  <si>
+    <t>Kyle Parker</t>
+  </si>
+  <si>
+    <t>Zach Walters</t>
+  </si>
+  <si>
+    <t>Kevin Pillar</t>
+  </si>
+  <si>
+    <t>Dylan Axelrod</t>
+  </si>
+  <si>
+    <t>Cory Luebke</t>
+  </si>
+  <si>
+    <t>Freddy Galvis</t>
+  </si>
+  <si>
+    <t>Alberto Callaspo</t>
+  </si>
+  <si>
+    <t>Stephen Piscotty</t>
+  </si>
+  <si>
+    <t>Chase Anderson</t>
+  </si>
+  <si>
+    <t>Guillermo Heredia</t>
+  </si>
+  <si>
+    <t>Justin Ruggiano</t>
+  </si>
+  <si>
+    <t>Alex Jackson</t>
+  </si>
+  <si>
+    <t>Mark Canha</t>
+  </si>
+  <si>
+    <t>Alex Guerrero</t>
+  </si>
+  <si>
+    <t>Eduardo Escobar</t>
+  </si>
+  <si>
+    <t>Jarred Cosart</t>
+  </si>
+  <si>
+    <t>Chris Taylor</t>
+  </si>
+  <si>
+    <t>John Axford</t>
+  </si>
+  <si>
+    <t>Vance Worley</t>
+  </si>
+  <si>
+    <t>D.J. Peterson</t>
+  </si>
+  <si>
+    <t>Danny Farquhar</t>
+  </si>
+  <si>
+    <t>Yasmany Tomas</t>
+  </si>
+  <si>
+    <t>Craig Gentry</t>
   </si>
 </sst>
 </file>
@@ -2597,10 +2672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D554"/>
+  <dimension ref="A1:D579"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B491" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B509" sqref="B509"/>
+    <sheetView tabSelected="1" topLeftCell="A561" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D566" sqref="D566"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6281,7 +6356,7 @@
         <v>263</v>
       </c>
       <c r="B263" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C263">
         <v>4</v>
@@ -7079,7 +7154,7 @@
         <v>179</v>
       </c>
       <c r="B320" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C320">
         <v>18</v>
@@ -7387,7 +7462,7 @@
         <v>59</v>
       </c>
       <c r="B342" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C342">
         <v>1</v>
@@ -9207,7 +9282,7 @@
         <v>201</v>
       </c>
       <c r="B472" t="s">
-        <v>499</v>
+        <v>608</v>
       </c>
       <c r="C472">
         <v>17</v>
@@ -9221,7 +9296,7 @@
         <v>146</v>
       </c>
       <c r="B473" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C473">
         <v>8</v>
@@ -9235,7 +9310,7 @@
         <v>4</v>
       </c>
       <c r="B474" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C474">
         <v>0</v>
@@ -9249,7 +9324,7 @@
         <v>216</v>
       </c>
       <c r="B475" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C475">
         <v>0</v>
@@ -9263,7 +9338,7 @@
         <v>108</v>
       </c>
       <c r="B476" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C476">
         <v>0</v>
@@ -9277,7 +9352,7 @@
         <v>278</v>
       </c>
       <c r="B477" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C477">
         <v>0</v>
@@ -9291,7 +9366,7 @@
         <v>120</v>
       </c>
       <c r="B478" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C478">
         <v>0</v>
@@ -9305,7 +9380,7 @@
         <v>120</v>
       </c>
       <c r="B479" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C479">
         <v>0</v>
@@ -9319,7 +9394,7 @@
         <v>43</v>
       </c>
       <c r="B480" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C480">
         <v>0</v>
@@ -9333,7 +9408,7 @@
         <v>201</v>
       </c>
       <c r="B481" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C481">
         <v>0</v>
@@ -9347,7 +9422,7 @@
         <v>278</v>
       </c>
       <c r="B482" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C482">
         <v>0</v>
@@ -9361,7 +9436,7 @@
         <v>26</v>
       </c>
       <c r="B483" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C483">
         <v>0</v>
@@ -9375,7 +9450,7 @@
         <v>249</v>
       </c>
       <c r="B484" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C484">
         <v>0</v>
@@ -9389,7 +9464,7 @@
         <v>146</v>
       </c>
       <c r="B485" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C485">
         <v>0</v>
@@ -9403,7 +9478,7 @@
         <v>216</v>
       </c>
       <c r="B486" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C486">
         <v>0</v>
@@ -9417,7 +9492,7 @@
         <v>4</v>
       </c>
       <c r="B487" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C487">
         <v>0</v>
@@ -9431,7 +9506,7 @@
         <v>4</v>
       </c>
       <c r="B488" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C488">
         <v>0</v>
@@ -9445,7 +9520,7 @@
         <v>216</v>
       </c>
       <c r="B489" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C489">
         <v>0</v>
@@ -9459,7 +9534,7 @@
         <v>108</v>
       </c>
       <c r="B490" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C490">
         <v>0</v>
@@ -9473,7 +9548,7 @@
         <v>108</v>
       </c>
       <c r="B491" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C491">
         <v>0</v>
@@ -9487,7 +9562,7 @@
         <v>249</v>
       </c>
       <c r="B492" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C492">
         <v>0</v>
@@ -9501,7 +9576,7 @@
         <v>26</v>
       </c>
       <c r="B493" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C493">
         <v>0</v>
@@ -9515,7 +9590,7 @@
         <v>230</v>
       </c>
       <c r="B494" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C494">
         <v>0</v>
@@ -9529,7 +9604,7 @@
         <v>74</v>
       </c>
       <c r="B495" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C495">
         <v>0</v>
@@ -9543,7 +9618,7 @@
         <v>278</v>
       </c>
       <c r="B496" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C496">
         <v>0</v>
@@ -9557,7 +9632,7 @@
         <v>146</v>
       </c>
       <c r="B497" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C497">
         <v>0</v>
@@ -9571,7 +9646,7 @@
         <v>59</v>
       </c>
       <c r="B498" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C498">
         <v>0</v>
@@ -9585,7 +9660,7 @@
         <v>179</v>
       </c>
       <c r="B499" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C499">
         <v>0</v>
@@ -9599,7 +9674,7 @@
         <v>91</v>
       </c>
       <c r="B500" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C500">
         <v>0</v>
@@ -9613,7 +9688,7 @@
         <v>201</v>
       </c>
       <c r="B501" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C501">
         <v>0</v>
@@ -9627,7 +9702,7 @@
         <v>263</v>
       </c>
       <c r="B502" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C502">
         <v>0</v>
@@ -9641,7 +9716,7 @@
         <v>120</v>
       </c>
       <c r="B503" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C503">
         <v>0</v>
@@ -9655,7 +9730,7 @@
         <v>164</v>
       </c>
       <c r="B504" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C504">
         <v>0</v>
@@ -9669,7 +9744,7 @@
         <v>43</v>
       </c>
       <c r="B505" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C505">
         <v>0</v>
@@ -9683,7 +9758,7 @@
         <v>43</v>
       </c>
       <c r="B506" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C506">
         <v>0</v>
@@ -9697,7 +9772,7 @@
         <v>164</v>
       </c>
       <c r="B507" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C507">
         <v>0</v>
@@ -9711,7 +9786,7 @@
         <v>120</v>
       </c>
       <c r="B508" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C508">
         <v>0</v>
@@ -9725,7 +9800,7 @@
         <v>263</v>
       </c>
       <c r="B509" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C509">
         <v>0</v>
@@ -9739,7 +9814,7 @@
         <v>146</v>
       </c>
       <c r="B510" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C510">
         <v>0</v>
@@ -9753,7 +9828,7 @@
         <v>201</v>
       </c>
       <c r="B511" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C511">
         <v>0</v>
@@ -9767,7 +9842,7 @@
         <v>91</v>
       </c>
       <c r="B512" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C512">
         <v>0</v>
@@ -9781,7 +9856,7 @@
         <v>179</v>
       </c>
       <c r="B513" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C513">
         <v>0</v>
@@ -9795,7 +9870,7 @@
         <v>59</v>
       </c>
       <c r="B514" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C514">
         <v>0</v>
@@ -9809,7 +9884,7 @@
         <v>278</v>
       </c>
       <c r="B515" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C515">
         <v>0</v>
@@ -9823,7 +9898,7 @@
         <v>74</v>
       </c>
       <c r="B516" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C516">
         <v>0</v>
@@ -9837,7 +9912,7 @@
         <v>230</v>
       </c>
       <c r="B517" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C517">
         <v>0</v>
@@ -9851,7 +9926,7 @@
         <v>26</v>
       </c>
       <c r="B518" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C518">
         <v>0</v>
@@ -9865,7 +9940,7 @@
         <v>249</v>
       </c>
       <c r="B519" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C519">
         <v>0</v>
@@ -9879,7 +9954,7 @@
         <v>108</v>
       </c>
       <c r="B520" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C520">
         <v>0</v>
@@ -9893,7 +9968,7 @@
         <v>146</v>
       </c>
       <c r="B521" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C521">
         <v>0</v>
@@ -9907,7 +9982,7 @@
         <v>216</v>
       </c>
       <c r="B522" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C522">
         <v>0</v>
@@ -9921,7 +9996,7 @@
         <v>4</v>
       </c>
       <c r="B523" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C523">
         <v>0</v>
@@ -9935,7 +10010,7 @@
         <v>4</v>
       </c>
       <c r="B524" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C524">
         <v>0</v>
@@ -9949,7 +10024,7 @@
         <v>216</v>
       </c>
       <c r="B525" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C525">
         <v>0</v>
@@ -9963,7 +10038,7 @@
         <v>146</v>
       </c>
       <c r="B526" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C526">
         <v>0</v>
@@ -9974,10 +10049,10 @@
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
-        <v>249</v>
+        <v>108</v>
       </c>
       <c r="B527" t="s">
-        <v>556</v>
+        <v>609</v>
       </c>
       <c r="C527">
         <v>0</v>
@@ -9988,10 +10063,10 @@
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
-        <v>26</v>
+        <v>249</v>
       </c>
       <c r="B528" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C528">
         <v>0</v>
@@ -10002,38 +10077,38 @@
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
-        <v>230</v>
+        <v>26</v>
       </c>
       <c r="B529" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C529">
         <v>0</v>
       </c>
       <c r="D529" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
-        <v>74</v>
+        <v>230</v>
       </c>
       <c r="B530" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C530">
         <v>0</v>
       </c>
       <c r="D530" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
-        <v>278</v>
+        <v>74</v>
       </c>
       <c r="B531" t="s">
-        <v>582</v>
+        <v>558</v>
       </c>
       <c r="C531">
         <v>0</v>
@@ -10044,10 +10119,10 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
-        <v>59</v>
+        <v>278</v>
       </c>
       <c r="B532" t="s">
-        <v>560</v>
+        <v>581</v>
       </c>
       <c r="C532">
         <v>0</v>
@@ -10058,10 +10133,10 @@
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
-        <v>179</v>
+        <v>59</v>
       </c>
       <c r="B533" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C533">
         <v>0</v>
@@ -10072,10 +10147,10 @@
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="B534" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C534">
         <v>0</v>
@@ -10086,10 +10161,10 @@
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="B535" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C535">
         <v>0</v>
@@ -10100,10 +10175,10 @@
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
-        <v>263</v>
+        <v>201</v>
       </c>
       <c r="B536" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C536">
         <v>0</v>
@@ -10114,10 +10189,10 @@
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="B537" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C537">
         <v>0</v>
@@ -10128,10 +10203,10 @@
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B538" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C538">
         <v>0</v>
@@ -10142,10 +10217,10 @@
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="B539" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C539">
         <v>0</v>
@@ -10156,10 +10231,10 @@
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="B540" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C540">
         <v>0</v>
@@ -10173,7 +10248,7 @@
         <v>43</v>
       </c>
       <c r="B541" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C541">
         <v>0</v>
@@ -10184,10 +10259,10 @@
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="B542" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C542">
         <v>0</v>
@@ -10198,10 +10273,10 @@
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
-        <v>120</v>
+        <v>164</v>
       </c>
       <c r="B543" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C543">
         <v>0</v>
@@ -10212,10 +10287,10 @@
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="B544" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C544">
         <v>0</v>
@@ -10226,10 +10301,10 @@
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
-        <v>263</v>
+        <v>146</v>
       </c>
       <c r="B545" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="C545">
         <v>0</v>
@@ -10240,10 +10315,10 @@
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="B546" t="s">
-        <v>573</v>
+        <v>582</v>
       </c>
       <c r="C546">
         <v>0</v>
@@ -10254,10 +10329,10 @@
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="B547" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C547">
         <v>0</v>
@@ -10268,10 +10343,10 @@
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
-        <v>179</v>
+        <v>91</v>
       </c>
       <c r="B548" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C548">
         <v>0</v>
@@ -10282,10 +10357,10 @@
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
-        <v>59</v>
+        <v>179</v>
       </c>
       <c r="B549" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C549">
         <v>0</v>
@@ -10296,10 +10371,10 @@
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
-        <v>278</v>
+        <v>59</v>
       </c>
       <c r="B550" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C550">
         <v>0</v>
@@ -10310,10 +10385,10 @@
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
-        <v>74</v>
+        <v>278</v>
       </c>
       <c r="B551" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C551">
         <v>0</v>
@@ -10324,10 +10399,10 @@
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
-        <v>230</v>
+        <v>74</v>
       </c>
       <c r="B552" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C552">
         <v>0</v>
@@ -10338,10 +10413,10 @@
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="B553" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C553">
         <v>0</v>
@@ -10352,15 +10427,365 @@
     </row>
     <row r="554" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
+        <v>26</v>
+      </c>
+      <c r="B554" t="s">
+        <v>579</v>
+      </c>
+      <c r="C554">
+        <v>0</v>
+      </c>
+      <c r="D554" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
         <v>249</v>
       </c>
-      <c r="B554" t="s">
-        <v>581</v>
-      </c>
-      <c r="C554">
-        <v>0</v>
-      </c>
-      <c r="D554" t="s">
+      <c r="B555" t="s">
+        <v>580</v>
+      </c>
+      <c r="C555">
+        <v>0</v>
+      </c>
+      <c r="D555" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>108</v>
+      </c>
+      <c r="B556" t="s">
+        <v>584</v>
+      </c>
+      <c r="C556">
+        <v>0</v>
+      </c>
+      <c r="D556" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>146</v>
+      </c>
+      <c r="B557" t="s">
+        <v>585</v>
+      </c>
+      <c r="C557">
+        <v>0</v>
+      </c>
+      <c r="D557" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>216</v>
+      </c>
+      <c r="B558" t="s">
+        <v>586</v>
+      </c>
+      <c r="C558">
+        <v>0</v>
+      </c>
+      <c r="D558" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>4</v>
+      </c>
+      <c r="B559" t="s">
+        <v>587</v>
+      </c>
+      <c r="C559">
+        <v>0</v>
+      </c>
+      <c r="D559" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>4</v>
+      </c>
+      <c r="B560" t="s">
+        <v>588</v>
+      </c>
+      <c r="C560">
+        <v>0</v>
+      </c>
+      <c r="D560" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>216</v>
+      </c>
+      <c r="B561" t="s">
+        <v>589</v>
+      </c>
+      <c r="C561">
+        <v>0</v>
+      </c>
+      <c r="D561" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>146</v>
+      </c>
+      <c r="B562" t="s">
+        <v>590</v>
+      </c>
+      <c r="C562">
+        <v>0</v>
+      </c>
+      <c r="D562" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>108</v>
+      </c>
+      <c r="B563" t="s">
+        <v>591</v>
+      </c>
+      <c r="C563">
+        <v>0</v>
+      </c>
+      <c r="D563" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>26</v>
+      </c>
+      <c r="B564" t="s">
+        <v>592</v>
+      </c>
+      <c r="C564">
+        <v>0</v>
+      </c>
+      <c r="D564" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>230</v>
+      </c>
+      <c r="B565" t="s">
+        <v>593</v>
+      </c>
+      <c r="C565">
+        <v>0</v>
+      </c>
+      <c r="D565" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>74</v>
+      </c>
+      <c r="B566" t="s">
+        <v>594</v>
+      </c>
+      <c r="C566">
+        <v>0</v>
+      </c>
+      <c r="D566" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>278</v>
+      </c>
+      <c r="B567" t="s">
+        <v>595</v>
+      </c>
+      <c r="C567">
+        <v>0</v>
+      </c>
+      <c r="D567" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>179</v>
+      </c>
+      <c r="B568" t="s">
+        <v>596</v>
+      </c>
+      <c r="C568">
+        <v>0</v>
+      </c>
+      <c r="D568" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>91</v>
+      </c>
+      <c r="B569" t="s">
+        <v>597</v>
+      </c>
+      <c r="C569">
+        <v>0</v>
+      </c>
+      <c r="D569" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>201</v>
+      </c>
+      <c r="B570" t="s">
+        <v>598</v>
+      </c>
+      <c r="C570">
+        <v>0</v>
+      </c>
+      <c r="D570" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>263</v>
+      </c>
+      <c r="B571" t="s">
+        <v>599</v>
+      </c>
+      <c r="C571">
+        <v>0</v>
+      </c>
+      <c r="D571" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>120</v>
+      </c>
+      <c r="B572" t="s">
+        <v>600</v>
+      </c>
+      <c r="C572">
+        <v>0</v>
+      </c>
+      <c r="D572" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>164</v>
+      </c>
+      <c r="B573" t="s">
+        <v>601</v>
+      </c>
+      <c r="C573">
+        <v>0</v>
+      </c>
+      <c r="D573" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>43</v>
+      </c>
+      <c r="B574" t="s">
+        <v>602</v>
+      </c>
+      <c r="C574">
+        <v>0</v>
+      </c>
+      <c r="D574" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>43</v>
+      </c>
+      <c r="B575" t="s">
+        <v>603</v>
+      </c>
+      <c r="C575">
+        <v>0</v>
+      </c>
+      <c r="D575" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>132</v>
+      </c>
+      <c r="B576" t="s">
+        <v>604</v>
+      </c>
+      <c r="C576">
+        <v>0</v>
+      </c>
+      <c r="D576" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>164</v>
+      </c>
+      <c r="B577" t="s">
+        <v>605</v>
+      </c>
+      <c r="C577">
+        <v>0</v>
+      </c>
+      <c r="D577" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>120</v>
+      </c>
+      <c r="B578" t="s">
+        <v>606</v>
+      </c>
+      <c r="C578">
+        <v>0</v>
+      </c>
+      <c r="D578" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>132</v>
+      </c>
+      <c r="B579" t="s">
+        <v>607</v>
+      </c>
+      <c r="C579">
+        <v>0</v>
+      </c>
+      <c r="D579" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>